<commit_message>
Move write_results function from p2p_parser to excel_writer
</commit_message>
<xml_diff>
--- a/tests/expected_results/result_test_write_results_bondora_no_cfs.xlsx
+++ b/tests/expected_results/result_test_write_results_bondora_no_cfs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tagesergebnisse" sheetId="1" state="visible" r:id="rId2"/>
@@ -214,16 +214,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.29"/>
@@ -279,7 +279,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -320,122 +320,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3" t="n">
-        <v>42644</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3" t="n">
-        <v>42675</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3" t="n">
-        <v>42705</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -460,7 +348,7 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.29"/>
@@ -689,14 +577,14 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.29"/>

</xml_diff>